<commit_message>
add Propellant Piston drawings
</commit_message>
<xml_diff>
--- a/PurchaseItems.xlsx
+++ b/PurchaseItems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Rocketry\liquid-halfCat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA7E530-7389-40EC-931D-7216527DAD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D1D1EB-52B1-4B5C-B671-E7D5802C237A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1830" windowWidth="24240" windowHeight="13020" tabRatio="599" xr2:uid="{8D159CE3-F855-4C47-BCD8-824ABD2B10DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{8D159CE3-F855-4C47-BCD8-824ABD2B10DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="372">
   <si>
     <t>Item</t>
   </si>
@@ -1103,6 +1103,60 @@
   </si>
   <si>
     <t>https://www.amazon.com/Splitter-Connector-Extension-Compatible-Airplanes/dp/B09VNQPP91?crid=3MAJU0RK53ZAK&amp;dib=eyJ2IjoiMSJ9.3gf6ef_DWLQUS_bMBdzBSTu4dobYQK0j9Fs4Xhy9Ud3t8GcEnYmE8bsj3X8Z8ztuwDi84HL1Owe9c_rKRE_Spg8NJxSfxbdVsp8QUMrwAsfNg_Ln4VQVY0Q0jP_r3rYiKjTouXB4jTmWD9bzZ4FsqbGN1H5RZUWxN05gVWIiDGqlFNU7xEPaMM0oyQHDWX2wEfgpL2L0lYm-6yyW_OAhZ5jqPE7gXVI1TiF8o-fphdjuwR2JLZXhcVRLM0BbNLYLLmGjo--PWKqSR06iPn5GwDPvDyI8HXDXwVzo93vJcEw.eJ8-VDxkjdvzrES9ReOmFuj4j5di6HF2HTIwzSTGbhQ</t>
+  </si>
+  <si>
+    <t>T-18</t>
+  </si>
+  <si>
+    <t>To be cut/machined into FLNG-ST-25T-8X250C</t>
+  </si>
+  <si>
+    <t>T-19</t>
+  </si>
+  <si>
+    <t>To be cut/machined into BRKT-90A-125T-2X250C</t>
+  </si>
+  <si>
+    <t>T-20</t>
+  </si>
+  <si>
+    <t>To be cut/machined into BKHD-REC-4X250C-2X170WE</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/88895k86/</t>
+  </si>
+  <si>
+    <t>88895K86</t>
+  </si>
+  <si>
+    <t>3/16" 5052 H32 Aluminum Plate 4"x24" (3x 4" OD)</t>
+  </si>
+  <si>
+    <t>1/8" 5052 H32 Aluminum Plate  2"x24" (8x 2.5x1)</t>
+  </si>
+  <si>
+    <t>9135K26-9135K262</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/9135K26-9135K262/</t>
+  </si>
+  <si>
+    <t>8910K587-8910K588</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/8910K587-8910K588/</t>
+  </si>
+  <si>
+    <t>1/4" Carbon Steel Plate 4.5"x12" (2x 4"OD)</t>
+  </si>
+  <si>
+    <t>To be cut/machined into 2x FLNG-ST-25T-8X250C</t>
+  </si>
+  <si>
+    <t>To be cut/machined into 8x BRKT-90A-125T-2X250C</t>
+  </si>
+  <si>
+    <t>To be cut/machined into 3x BKHD-REC-4X250C-2X170WE</t>
   </si>
 </sst>
 </file>
@@ -1367,10 +1421,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89D6DB8E-A063-40CC-A8B4-CCDB1855DD3B}" name="Table1" displayName="Table1" ref="A1:J72" totalsRowShown="0">
-  <autoFilter ref="A1:J72" xr:uid="{89D6DB8E-A063-40CC-A8B4-CCDB1855DD3B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J72">
-    <sortCondition descending="1" ref="C1:C72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89D6DB8E-A063-40CC-A8B4-CCDB1855DD3B}" name="Table1" displayName="Table1" ref="A1:J75" totalsRowShown="0">
+  <autoFilter ref="A1:J75" xr:uid="{89D6DB8E-A063-40CC-A8B4-CCDB1855DD3B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J75">
+    <sortCondition descending="1" ref="C1:C75"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3A11ACE5-9142-412A-81D3-C9031012649E}" name="Number" dataDxfId="9"/>
@@ -1707,11 +1761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F63C74-907A-4605-A86F-6C239F74206D}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,215 +2177,225 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>34</v>
+        <v>354</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>367</v>
       </c>
       <c r="F14" s="13">
-        <v>17.600000000000001</v>
+        <v>34.86</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
       </c>
       <c r="H14" s="13">
         <f>F14*G14</f>
-        <v>17.600000000000001</v>
+        <v>34.86</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>55</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>77</v>
+        <v>356</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>92</v>
+        <v>361</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>115</v>
+        <v>360</v>
       </c>
       <c r="F15" s="13">
-        <v>2.58</v>
+        <v>17.2</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>
       </c>
       <c r="H15" s="13">
         <f>F15*G15</f>
-        <v>2.58</v>
+        <v>17.2</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>180</v>
+        <v>358</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>205</v>
+        <v>364</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>223</v>
+        <v>365</v>
       </c>
       <c r="F16" s="13">
-        <v>10.17</v>
+        <v>38.72</v>
       </c>
       <c r="G16" s="8">
         <v>1</v>
       </c>
       <c r="H16" s="13">
         <f>F16*G16</f>
-        <v>10.17</v>
+        <v>38.72</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>191</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>271</v>
+        <v>278</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="13">
+        <v>17.600000000000001</v>
       </c>
       <c r="G17" s="8">
-        <v>2</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <f>F17*G17</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>32</v>
+        <v>304</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="13">
+        <v>2.58</v>
       </c>
       <c r="G18" s="8">
         <v>1</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>51</v>
+      <c r="H18" s="13">
+        <f>F18*G18</f>
+        <v>2.58</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>79</v>
+        <v>329</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>271</v>
+        <v>349</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>51</v>
+        <v>205</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F19" s="13">
+        <v>10.17</v>
       </c>
       <c r="G19" s="8">
         <v>1</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>51</v>
+      <c r="H19" s="13">
+        <f>F19*G19</f>
+        <v>10.17</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>143</v>
+        <v>286</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>271</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="12"/>
+        <v>49</v>
+      </c>
       <c r="F20" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>175</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>144</v>
+        <v>287</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>271</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" s="12"/>
+        <v>50</v>
+      </c>
       <c r="F21" s="13" t="s">
         <v>51</v>
       </c>
@@ -2342,373 +2406,357 @@
         <v>51</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>175</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
+        <v>306</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="13">
-        <v>7.88</v>
+        <v>94</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G22" s="8">
         <v>1</v>
       </c>
-      <c r="H22" s="13">
-        <f>F22*G22</f>
-        <v>7.88</v>
+      <c r="H22" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>25</v>
+        <v>322</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="13">
-        <v>9.2100000000000009</v>
+        <v>146</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G23" s="8">
         <v>1</v>
       </c>
-      <c r="H23" s="13">
-        <f>F23*G23</f>
-        <v>9.2100000000000009</v>
+      <c r="H23" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>26</v>
+        <v>323</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="13">
-        <v>9.3000000000000007</v>
+        <v>145</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G24" s="8">
         <v>1</v>
       </c>
-      <c r="H24" s="13">
-        <f>F24*G24</f>
-        <v>9.3000000000000007</v>
+      <c r="H24" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>58</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F25" s="13">
-        <v>0.39</v>
+        <v>7.88</v>
       </c>
       <c r="G25" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="13">
         <f>F25*G25</f>
-        <v>0.78</v>
+        <v>7.88</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F26" s="13">
-        <v>7.49</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G26" s="8">
         <v>1</v>
       </c>
       <c r="H26" s="13">
         <f>F26*G26</f>
-        <v>7.49</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F27" s="13">
-        <v>5.23</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G27" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="13">
         <f>F27*G27</f>
-        <v>10.46</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F28" s="13">
-        <v>4.3099999999999996</v>
+        <v>0.39</v>
       </c>
       <c r="G28" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="13">
         <f>F28*G28</f>
-        <v>4.3099999999999996</v>
+        <v>0.78</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="F29" s="13">
-        <v>2.02</v>
+        <v>7.49</v>
       </c>
       <c r="G29" s="8">
         <v>1</v>
       </c>
       <c r="H29" s="13">
         <f>F29*G29</f>
-        <v>2.02</v>
+        <v>7.49</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>161</v>
+        <v>46</v>
       </c>
       <c r="F30" s="13">
-        <v>1.9</v>
+        <v>5.23</v>
       </c>
       <c r="G30" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="13">
         <f>F30*G30</f>
-        <v>1.9</v>
+        <v>10.46</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>133</v>
+        <v>285</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="F31" s="13">
-        <v>3.98</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="G31" s="8">
         <v>1</v>
       </c>
       <c r="H31" s="13">
         <f>F31*G31</f>
-        <v>3.98</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>170</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>135</v>
+        <v>312</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F32" s="13">
-        <v>10.56</v>
+        <v>2.02</v>
       </c>
       <c r="G32" s="8">
         <v>1</v>
       </c>
       <c r="H32" s="13">
         <f>F32*G32</f>
-        <v>10.56</v>
+        <v>2.02</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>138</v>
+        <v>313</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F33" s="13">
-        <v>3.43</v>
+        <v>1.9</v>
       </c>
       <c r="G33" s="8">
         <v>1</v>
       </c>
       <c r="H33" s="13">
         <f>F33*G33</f>
-        <v>3.43</v>
+        <v>1.9</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>171</v>
@@ -2719,98 +2767,95 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>137</v>
+        <v>314</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F34" s="13">
-        <v>1.94</v>
+        <v>3.98</v>
       </c>
       <c r="G34" s="8">
         <v>1</v>
       </c>
       <c r="H34" s="13">
         <f>F34*G34</f>
-        <v>1.94</v>
+        <v>3.98</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F35" s="13">
-        <v>2.19</v>
+        <v>10.56</v>
       </c>
       <c r="G35" s="8">
         <v>1</v>
       </c>
       <c r="H35" s="13">
         <f>F35*G35</f>
-        <v>2.19</v>
+        <v>10.56</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J35" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F36" s="13">
-        <v>2.2799999999999998</v>
+        <v>3.43</v>
       </c>
       <c r="G36" s="8">
         <v>1</v>
       </c>
       <c r="H36" s="13">
         <f>F36*G36</f>
-        <v>2.2799999999999998</v>
+        <v>3.43</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>134</v>
@@ -2818,1185 +2863,1287 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>237</v>
+        <v>164</v>
       </c>
       <c r="F37" s="13">
-        <v>1.27</v>
+        <v>1.94</v>
       </c>
       <c r="G37" s="8">
         <v>1</v>
       </c>
       <c r="H37" s="13">
         <f>F37*G37</f>
-        <v>1.27</v>
+        <v>1.94</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>192</v>
+        <v>171</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="F38" s="13">
-        <v>3.11</v>
+        <v>2.19</v>
       </c>
       <c r="G38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38" s="13">
         <f>F38*G38</f>
-        <v>6.22</v>
+        <v>2.19</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F39" s="13">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G39" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="13">
         <f>F39*G39</f>
-        <v>0</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>238</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
+        <v>206</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" s="13">
+        <v>1.27</v>
+      </c>
       <c r="G40" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H40" s="13">
         <f>F40*G40</f>
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F41" s="13">
-        <v>5.5</v>
+        <v>3.11</v>
       </c>
       <c r="G41" s="8">
         <v>2</v>
       </c>
       <c r="H41" s="13">
         <f>F41*G41</f>
-        <v>11</v>
+        <v>6.22</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="F42" s="13">
-        <v>3.02</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42" s="13">
         <f>F42*G42</f>
-        <v>3.02</v>
+        <v>0</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="F43" s="13">
-        <v>7.08</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H43" s="13">
         <f>F43*G43</f>
-        <v>7.08</v>
+        <v>0</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F44" s="13">
-        <v>2.46</v>
+        <v>5.5</v>
       </c>
       <c r="G44" s="8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H44" s="13">
         <f>F44*G44</f>
-        <v>19.68</v>
+        <v>11</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>239</v>
+        <v>185</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F45" s="13">
-        <v>7.93</v>
+        <v>3.02</v>
       </c>
       <c r="G45" s="8">
         <v>1</v>
       </c>
       <c r="H45" s="13">
         <f>F45*G45</f>
-        <v>7.93</v>
+        <v>3.02</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C46" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>270</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F46" s="13">
-        <v>1.07</v>
+        <v>7.08</v>
       </c>
       <c r="G46" s="8">
         <v>1</v>
       </c>
       <c r="H46" s="13">
         <f>F46*G46</f>
-        <v>1.07</v>
+        <v>7.08</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>188</v>
+        <v>337</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>231</v>
+      <c r="D47" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="F47" s="13">
-        <v>6.32</v>
+        <v>2.46</v>
       </c>
       <c r="G47" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H47" s="13">
         <f>F47*G47</f>
-        <v>6.32</v>
+        <v>19.68</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>62</v>
+        <v>338</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>239</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>307</v>
+        <v>270</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>81</v>
+        <v>212</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>107</v>
+        <v>229</v>
       </c>
       <c r="F48" s="13">
-        <v>6.97</v>
+        <v>7.93</v>
       </c>
       <c r="G48" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H48" s="13">
         <f>F48*G48</f>
-        <v>13.94</v>
+        <v>7.93</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>307</v>
+        <v>339</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>82</v>
+        <v>213</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>108</v>
+        <v>230</v>
       </c>
       <c r="F49" s="13">
-        <v>3.25</v>
+        <v>1.07</v>
       </c>
       <c r="G49" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H49" s="13">
         <f>F49*G49</f>
-        <v>6.5</v>
+        <v>1.07</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>64</v>
+        <v>340</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>109</v>
+        <v>270</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>231</v>
       </c>
       <c r="F50" s="13">
-        <v>2.64</v>
+        <v>6.32</v>
       </c>
       <c r="G50" s="8">
         <v>1</v>
       </c>
       <c r="H50" s="13">
         <f>F50*G50</f>
-        <v>2.64</v>
+        <v>6.32</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F51" s="13">
-        <v>3.31</v>
+        <v>6.97</v>
       </c>
       <c r="G51" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51" s="13">
         <f>F51*G51</f>
-        <v>3.31</v>
+        <v>13.94</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F52" s="13">
-        <v>5.38</v>
+        <v>3.25</v>
       </c>
       <c r="G52" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H52" s="13">
         <f>F52*G52</f>
-        <v>5.38</v>
+        <v>6.5</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>70</v>
+        <v>290</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F53" s="13">
-        <v>4.47</v>
+        <v>2.64</v>
       </c>
       <c r="G53" s="8">
         <v>1</v>
       </c>
       <c r="H53" s="13">
         <f>F53*G53</f>
-        <v>4.47</v>
+        <v>2.64</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>71</v>
+        <v>289</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F54" s="13">
-        <v>3.65</v>
+        <v>3.31</v>
       </c>
       <c r="G54" s="8">
         <v>1</v>
       </c>
       <c r="H54" s="13">
         <f>F54*G54</f>
-        <v>3.65</v>
+        <v>3.31</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>307</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F55" s="13">
-        <v>19.260000000000002</v>
+        <v>5.38</v>
       </c>
       <c r="G55" s="8">
         <v>1</v>
       </c>
       <c r="H55" s="13">
         <f>F55*G55</f>
-        <v>19.260000000000002</v>
+        <v>5.38</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F56" s="13">
-        <v>2.16</v>
+        <v>4.47</v>
       </c>
       <c r="G56" s="8">
         <v>1</v>
       </c>
       <c r="H56" s="13">
         <f>F56*G56</f>
-        <v>2.16</v>
+        <v>4.47</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F57" s="13">
-        <v>3.95</v>
+        <v>3.65</v>
       </c>
       <c r="G57" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H57" s="13">
         <f>F57*G57</f>
-        <v>7.9</v>
+        <v>3.65</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F58" s="13">
-        <v>2.66</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="G58" s="8">
         <v>1</v>
       </c>
       <c r="H58" s="13">
         <f>F58*G58</f>
-        <v>2.66</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>131</v>
+        <v>301</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="F59" s="13">
-        <v>17.260000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="G59" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H59" s="13">
         <f>F59*G59</f>
-        <v>34.520000000000003</v>
+        <v>2.16</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>66</v>
+        <v>302</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>236</v>
+        <v>114</v>
       </c>
       <c r="F60" s="13">
-        <v>5.38</v>
+        <v>3.95</v>
       </c>
       <c r="G60" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H60" s="13">
         <f>F60*G60</f>
-        <v>5.38</v>
+        <v>7.9</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>179</v>
+        <v>305</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>204</v>
+        <v>93</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>222</v>
+        <v>116</v>
       </c>
       <c r="F61" s="13">
-        <v>5.18</v>
+        <v>2.66</v>
       </c>
       <c r="G61" s="8">
         <v>1</v>
       </c>
       <c r="H61" s="13">
         <f>F61*G61</f>
-        <v>5.18</v>
+        <v>2.66</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>261</v>
+        <v>131</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>252</v>
+        <v>148</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>260</v>
+        <v>159</v>
       </c>
       <c r="F62" s="13">
-        <v>11.27</v>
+        <v>17.260000000000002</v>
       </c>
       <c r="G62" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62" s="13">
         <f>F62*G62</f>
-        <v>11.27</v>
+        <v>34.520000000000003</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>248</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>240</v>
+        <v>66</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>253</v>
+        <v>85</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="F63" s="13">
-        <v>2.96</v>
+        <v>5.38</v>
       </c>
       <c r="G63" s="8">
         <v>1</v>
       </c>
       <c r="H63" s="13">
         <f>F63*G63</f>
-        <v>2.96</v>
+        <v>5.38</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>241</v>
+        <v>328</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>179</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>254</v>
+        <v>204</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>263</v>
+        <v>222</v>
       </c>
       <c r="F64" s="13">
-        <v>4.05</v>
+        <v>5.18</v>
       </c>
       <c r="G64" s="8">
         <v>1</v>
       </c>
       <c r="H64" s="13">
         <f>F64*G64</f>
-        <v>4.05</v>
+        <v>5.18</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>248</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F65" s="13">
-        <v>4.72</v>
+        <v>11.27</v>
       </c>
       <c r="G65" s="8">
         <v>1</v>
       </c>
       <c r="H65" s="13">
         <f>F65*G65</f>
-        <v>4.72</v>
+        <v>11.27</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>243</v>
+        <v>342</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F66" s="13">
-        <v>3.32</v>
+        <v>2.96</v>
       </c>
       <c r="G66" s="8">
         <v>1</v>
       </c>
       <c r="H66" s="13">
         <f>F66*G66</f>
-        <v>3.32</v>
+        <v>2.96</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>244</v>
+        <v>344</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>241</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F67" s="13">
-        <v>1.4</v>
+        <v>4.05</v>
       </c>
       <c r="G67" s="8">
         <v>1</v>
       </c>
       <c r="H67" s="13">
         <f>F67*G67</f>
-        <v>1.4</v>
+        <v>4.05</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>245</v>
+        <v>343</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F68" s="13">
-        <v>1.66</v>
+        <v>4.72</v>
       </c>
       <c r="G68" s="8">
         <v>1</v>
       </c>
       <c r="H68" s="13">
         <f>F68*G68</f>
-        <v>1.66</v>
+        <v>4.72</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>246</v>
+        <v>345</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>243</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F69" s="13">
-        <v>1.46</v>
+        <v>3.32</v>
       </c>
       <c r="G69" s="8">
         <v>1</v>
       </c>
       <c r="H69" s="13">
         <f>F69*G69</f>
-        <v>1.46</v>
+        <v>3.32</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>130</v>
+        <v>346</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>244</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>351</v>
+        <v>266</v>
       </c>
       <c r="F70" s="13">
-        <v>28.88</v>
+        <v>1.4</v>
       </c>
       <c r="G70" s="8">
         <v>1</v>
       </c>
       <c r="H70" s="13">
         <f>F70*G70</f>
-        <v>28.88</v>
+        <v>1.4</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>168</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>141</v>
+        <v>245</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>352</v>
+        <v>267</v>
       </c>
       <c r="F71" s="13">
-        <v>11.99</v>
+        <v>1.66</v>
       </c>
       <c r="G71" s="8">
         <v>1</v>
       </c>
       <c r="H71" s="13">
         <f>F71*G71</f>
-        <v>11.99</v>
+        <v>1.66</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>142</v>
+        <v>246</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>158</v>
+        <v>259</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>353</v>
+        <v>268</v>
       </c>
       <c r="F72" s="13">
-        <v>8.99</v>
+        <v>1.46</v>
       </c>
       <c r="G72" s="8">
         <v>1</v>
       </c>
       <c r="H72" s="13">
         <f>F72*G72</f>
+        <v>1.46</v>
+      </c>
+      <c r="I72" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F73" s="13">
+        <v>28.88</v>
+      </c>
+      <c r="G73" s="8">
+        <v>1</v>
+      </c>
+      <c r="H73" s="13">
+        <f>F73*G73</f>
+        <v>28.88</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="F74" s="13">
+        <v>11.99</v>
+      </c>
+      <c r="G74" s="8">
+        <v>1</v>
+      </c>
+      <c r="H74" s="13">
+        <f>F74*G74</f>
+        <v>11.99</v>
+      </c>
+      <c r="I74" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="F75" s="13">
         <v>8.99</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="13"/>
-      <c r="F73" s="13"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="G75" s="8">
+        <v>1</v>
+      </c>
+      <c r="H75" s="13">
+        <f>F75*G75</f>
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="9"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="13"/>
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="13">
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="13">
         <f>SUM(Table1[Cost])</f>
-        <v>787.26999999999987</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="13"/>
-      <c r="F75" s="13"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F77" s="13"/>
+        <v>878.04999999999984</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="13"/>
+      <c r="F78" s="13"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F80" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A77:G77"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{4C4F83D5-CAF2-4782-A95F-6ABBBE5C03D0}"/>
     <hyperlink ref="E7" r:id="rId2" xr:uid="{6A9DC51E-66FC-4B5D-B242-7F1F803F5F47}"/>
     <hyperlink ref="E8" r:id="rId3" xr:uid="{5290A744-9FD0-4E16-84EE-CECBE2D27A36}"/>
     <hyperlink ref="E9" r:id="rId4" xr:uid="{C67A8462-8BA2-4A5E-97DB-0BEECD6393A8}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{71CB020E-B9D8-4ECA-9672-E24809226AC9}"/>
-    <hyperlink ref="E22" r:id="rId6" xr:uid="{E7A2AACB-C950-45EB-AF7D-D4E17F491AC4}"/>
-    <hyperlink ref="E23" r:id="rId7" xr:uid="{18BC1D41-AAD7-47F5-893E-500BD5A2FC97}"/>
-    <hyperlink ref="E24" r:id="rId8" xr:uid="{A1F1F232-255C-48C4-BC79-6CE60D5DD10C}"/>
-    <hyperlink ref="E25" r:id="rId9" xr:uid="{75468C36-B2BA-43B8-8C7C-F7910208ABA3}"/>
-    <hyperlink ref="E26" r:id="rId10" xr:uid="{1C0B9B3C-EA28-49B6-8258-5BC4F88B094B}"/>
-    <hyperlink ref="E27" r:id="rId11" xr:uid="{4472E034-1F89-4B9C-A486-1381F2BC4398}"/>
-    <hyperlink ref="E28" r:id="rId12" xr:uid="{69A5146D-6AC1-47D4-AE0F-89577509D92F}"/>
-    <hyperlink ref="E48" r:id="rId13" xr:uid="{4DF42524-9F52-4D5C-9DC2-7F190FE0D742}"/>
-    <hyperlink ref="E49" r:id="rId14" xr:uid="{95F00FCD-398C-44C7-AEA2-DF2BAADE169A}"/>
-    <hyperlink ref="E50" r:id="rId15" xr:uid="{2149098F-BAFA-43C6-9117-42CCD019E9A0}"/>
-    <hyperlink ref="E51" r:id="rId16" xr:uid="{A6FF63FD-1F37-4573-87C8-DFE6B9024FF7}"/>
-    <hyperlink ref="E52" r:id="rId17" xr:uid="{A8F50886-8FA3-4B6D-8F2A-DF9B81EC3AAB}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{71CB020E-B9D8-4ECA-9672-E24809226AC9}"/>
+    <hyperlink ref="E25" r:id="rId6" xr:uid="{E7A2AACB-C950-45EB-AF7D-D4E17F491AC4}"/>
+    <hyperlink ref="E26" r:id="rId7" xr:uid="{18BC1D41-AAD7-47F5-893E-500BD5A2FC97}"/>
+    <hyperlink ref="E27" r:id="rId8" xr:uid="{A1F1F232-255C-48C4-BC79-6CE60D5DD10C}"/>
+    <hyperlink ref="E28" r:id="rId9" xr:uid="{75468C36-B2BA-43B8-8C7C-F7910208ABA3}"/>
+    <hyperlink ref="E29" r:id="rId10" xr:uid="{1C0B9B3C-EA28-49B6-8258-5BC4F88B094B}"/>
+    <hyperlink ref="E30" r:id="rId11" xr:uid="{4472E034-1F89-4B9C-A486-1381F2BC4398}"/>
+    <hyperlink ref="E31" r:id="rId12" xr:uid="{69A5146D-6AC1-47D4-AE0F-89577509D92F}"/>
+    <hyperlink ref="E51" r:id="rId13" xr:uid="{4DF42524-9F52-4D5C-9DC2-7F190FE0D742}"/>
+    <hyperlink ref="E52" r:id="rId14" xr:uid="{95F00FCD-398C-44C7-AEA2-DF2BAADE169A}"/>
+    <hyperlink ref="E53" r:id="rId15" xr:uid="{2149098F-BAFA-43C6-9117-42CCD019E9A0}"/>
+    <hyperlink ref="E54" r:id="rId16" xr:uid="{A6FF63FD-1F37-4573-87C8-DFE6B9024FF7}"/>
+    <hyperlink ref="E55" r:id="rId17" xr:uid="{A8F50886-8FA3-4B6D-8F2A-DF9B81EC3AAB}"/>
     <hyperlink ref="E2" r:id="rId18" xr:uid="{21743BBB-4111-4F15-BE61-1EDAFE830E08}"/>
     <hyperlink ref="E3" r:id="rId19" xr:uid="{192CBCDC-6E23-4257-A84F-A129F82056E1}"/>
     <hyperlink ref="E4" r:id="rId20" xr:uid="{E12B9D38-40D0-4373-AB16-846EE4CDA224}"/>
-    <hyperlink ref="E53" r:id="rId21" xr:uid="{A7246765-FBC7-4958-ADA2-6ACB242A31F6}"/>
-    <hyperlink ref="E54" r:id="rId22" xr:uid="{D0A1B85E-160E-4511-BA97-76AFE8163665}"/>
+    <hyperlink ref="E56" r:id="rId21" xr:uid="{A7246765-FBC7-4958-ADA2-6ACB242A31F6}"/>
+    <hyperlink ref="E57" r:id="rId22" xr:uid="{D0A1B85E-160E-4511-BA97-76AFE8163665}"/>
     <hyperlink ref="E5" r:id="rId23" xr:uid="{5A11146E-84D0-4FB1-AC18-4211615BEC44}"/>
-    <hyperlink ref="E55" r:id="rId24" xr:uid="{16E39919-85B9-493E-9442-521CA888A0C0}"/>
-    <hyperlink ref="E56" r:id="rId25" xr:uid="{A19EAFD2-6E53-4663-89CB-5AFB9CF2EE16}"/>
-    <hyperlink ref="E57" r:id="rId26" xr:uid="{93FC5B00-8834-405E-BD7F-CE9FC9F0636C}"/>
+    <hyperlink ref="E58" r:id="rId24" xr:uid="{16E39919-85B9-493E-9442-521CA888A0C0}"/>
+    <hyperlink ref="E59" r:id="rId25" xr:uid="{A19EAFD2-6E53-4663-89CB-5AFB9CF2EE16}"/>
+    <hyperlink ref="E60" r:id="rId26" xr:uid="{93FC5B00-8834-405E-BD7F-CE9FC9F0636C}"/>
     <hyperlink ref="E10" r:id="rId27" xr:uid="{2A686785-FFFF-4FE3-99C1-FC7AFBB6FCAB}"/>
-    <hyperlink ref="E15" r:id="rId28" xr:uid="{03EE2DF2-4169-4A0E-B640-F525C955FBDB}"/>
-    <hyperlink ref="E58" r:id="rId29" xr:uid="{E67731C1-06AC-4B34-8369-EA43B331ED20}"/>
-    <hyperlink ref="E59" r:id="rId30" xr:uid="{70C07E1A-175B-4C06-B8C8-241662C2C88B}"/>
-    <hyperlink ref="E29" r:id="rId31" xr:uid="{BAC0196A-B489-41F5-B827-4F773126FFDD}"/>
-    <hyperlink ref="E30" r:id="rId32" xr:uid="{A5FD4359-4772-44A7-893A-B635C00AE3D5}"/>
-    <hyperlink ref="E31" r:id="rId33" xr:uid="{04BCC309-389A-421E-8F2F-337CC34414B2}"/>
-    <hyperlink ref="E32" r:id="rId34" xr:uid="{583C8DDE-3F0F-42D6-B4E9-7FF80C867FDC}"/>
-    <hyperlink ref="E33" r:id="rId35" xr:uid="{1CE5F069-DB97-402C-8165-CE23796C7F62}"/>
-    <hyperlink ref="E34" r:id="rId36" xr:uid="{63C4700C-BEEC-4629-A532-CE8106156761}"/>
-    <hyperlink ref="E35" r:id="rId37" xr:uid="{2665E0C5-9B63-4BAE-BBDC-06803C38C0AA}"/>
-    <hyperlink ref="E36" r:id="rId38" xr:uid="{D0375459-DF0D-434A-A072-653F20FE4EEA}"/>
+    <hyperlink ref="E18" r:id="rId28" xr:uid="{03EE2DF2-4169-4A0E-B640-F525C955FBDB}"/>
+    <hyperlink ref="E61" r:id="rId29" xr:uid="{E67731C1-06AC-4B34-8369-EA43B331ED20}"/>
+    <hyperlink ref="E62" r:id="rId30" xr:uid="{70C07E1A-175B-4C06-B8C8-241662C2C88B}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{BAC0196A-B489-41F5-B827-4F773126FFDD}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{A5FD4359-4772-44A7-893A-B635C00AE3D5}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{04BCC309-389A-421E-8F2F-337CC34414B2}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{583C8DDE-3F0F-42D6-B4E9-7FF80C867FDC}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{1CE5F069-DB97-402C-8165-CE23796C7F62}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{63C4700C-BEEC-4629-A532-CE8106156761}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{2665E0C5-9B63-4BAE-BBDC-06803C38C0AA}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{D0375459-DF0D-434A-A072-653F20FE4EEA}"/>
     <hyperlink ref="E11" r:id="rId39" xr:uid="{AE1FCF5D-E50B-4DB9-A999-5D97DF02C67F}"/>
     <hyperlink ref="E12" r:id="rId40" xr:uid="{99055D5C-DD91-45F4-AAEF-B611C1BB3922}"/>
     <hyperlink ref="E13" r:id="rId41" xr:uid="{72D87336-89F0-4C92-B51C-96A472F81229}"/>
-    <hyperlink ref="E60" r:id="rId42" xr:uid="{F4A25109-22B2-4774-8556-010A6432F45C}"/>
-    <hyperlink ref="E61" r:id="rId43" xr:uid="{56089546-10EB-4408-9A09-4DEBD7481848}"/>
-    <hyperlink ref="E16" r:id="rId44" xr:uid="{14589A0F-B504-4BE9-9AFE-5448BF150C87}"/>
-    <hyperlink ref="E37" r:id="rId45" xr:uid="{5723DA9D-D179-4AEB-AB95-294595786C74}"/>
-    <hyperlink ref="E38" r:id="rId46" xr:uid="{042DF449-509B-4AEA-9A35-77C1FB9C2735}"/>
-    <hyperlink ref="E41" r:id="rId47" xr:uid="{96328DC4-D284-4D83-BEF7-74DFDF600418}"/>
-    <hyperlink ref="E42" r:id="rId48" xr:uid="{DE36F8FF-4A6C-40BD-AAE6-2EED680C3898}"/>
-    <hyperlink ref="E43" r:id="rId49" xr:uid="{34A64F91-02F3-467E-BE15-CC86C3D830E3}"/>
-    <hyperlink ref="E44" r:id="rId50" xr:uid="{C7CFF23B-B4AD-4B40-AE34-2C736F0F2EEC}"/>
-    <hyperlink ref="E45" r:id="rId51" xr:uid="{D061E5B9-6B5D-4A8C-87DC-6AB1EFE918D9}"/>
-    <hyperlink ref="E46" r:id="rId52" xr:uid="{7E3C3772-744A-4671-863E-0AC0F3BC1DC4}"/>
-    <hyperlink ref="E47" r:id="rId53" xr:uid="{B7F14980-6546-4BA8-A7E9-12B0123B1973}"/>
-    <hyperlink ref="E62" r:id="rId54" xr:uid="{C03F301E-1DDE-43B9-96B0-8E626F826DD1}"/>
-    <hyperlink ref="E63" r:id="rId55" xr:uid="{C960EB57-8A4D-4F2C-B021-A2110DCDBFE6}"/>
-    <hyperlink ref="E64" r:id="rId56" xr:uid="{0F51C24B-5731-40DA-B3D9-7765B93C6025}"/>
-    <hyperlink ref="E65" r:id="rId57" xr:uid="{F267908B-A49A-4C91-A420-01096F7A73FB}"/>
-    <hyperlink ref="E66" r:id="rId58" xr:uid="{B16C09CA-B6D3-40FB-B5F6-0A74F113D147}"/>
-    <hyperlink ref="E67" r:id="rId59" xr:uid="{11FB9D27-1B25-4BD0-B30E-EA1605974124}"/>
-    <hyperlink ref="E68" r:id="rId60" xr:uid="{0D0EDC79-794C-4303-BD64-256E6390377A}"/>
-    <hyperlink ref="E69" r:id="rId61" xr:uid="{2CC32D6E-23AB-4957-BF43-727F4EEFCA7E}"/>
-    <hyperlink ref="E70" r:id="rId62" display="https://www.amazon.com/Miuzei-Waterproof-Compatible-Steering-Horn%EF%BC%88270%C2%B0%EF%BC%89/dp/B0C5LTKBD4?crid=2K8NLBN9K63XX&amp;dib=eyJ2IjoiMSJ9.n9l0Ww8Rh99Yx4hzyqJ9wSAyYPbGAZn5JMDhIOwhG3Uw9VdkAuhdsgHMtc7JHErXrmf3c268ZwFiHkeGe0ALflEUcg5wkIqvJz42MkQUS3bvyfMdTo_fCm8QV5itEJuxTHHOCoL7rykJ9owy7cODiUViszR0WHjpremcAmeUST13w_0mg2vkg4IgXuYQKZ7Ccs9oFabkHPIo3RM1o73uUMa3Behvkr31QSVdAIXbSvS7OLY_QLBOF2RP8fN9Xyg02z8P3gJxlLPofnqUuW03FaekBfju58afSh6dm8qpApI.WbTiyjsVeZwrAeYG6HzABV9sIZ-waYUxXiAkjk08HI8&amp;th=1" xr:uid="{1D0B1835-36B7-4E7A-848F-D949E2357CD4}"/>
-    <hyperlink ref="E71" r:id="rId63" display="https://www.amazon.com/Extension-Female-Connectors-Control-11-8In-15Pcs/dp/B0CG3CDQ94?crid=2081JSZ9MFZC1&amp;dib=eyJ2IjoiMSJ9.I7ZCJdlPJPsGhcKI302M1gm1hB9gbSQSY3NSu1xpA227bSCB24BUjDlVIGNF0ehsNOp8ZgfiAxO6nPkgPJidUHO6Fclu6tExIgcUKjUn2idqMO_uHKPGeZx9v9CaA0I2Juw_Fs4EiaU-4QZn82m0dlpbm3lBiUMpyrKhxjjBDDnv9wZVRSdjcYI37GiJM1Z8ESRUP8JmlbwT-exEMQZA0_nztRsRFG4qOIc5q5yEbHHTs0u8MraiDyI6jfmffO_vKCZB4cfFjDBUf9O3n2DpvBpkwN8pI-octMZbU1UVzT4.c_1Xt0QKON6To9mY2iIk-0Bfv5-USH13yYJAGg_KwBo" xr:uid="{3BA4891F-C4E0-4EBC-B725-FD3CC8460AC6}"/>
-    <hyperlink ref="E72" r:id="rId64" display="https://www.amazon.com/Splitter-Connector-Extension-Compatible-Airplanes/dp/B09VNQPP91?crid=3MAJU0RK53ZAK&amp;dib=eyJ2IjoiMSJ9.3gf6ef_DWLQUS_bMBdzBSTu4dobYQK0j9Fs4Xhy9Ud3t8GcEnYmE8bsj3X8Z8ztuwDi84HL1Owe9c_rKRE_Spg8NJxSfxbdVsp8QUMrwAsfNg_Ln4VQVY0Q0jP_r3rYiKjTouXB4jTmWD9bzZ4FsqbGN1H5RZUWxN05gVWIiDGqlFNU7xEPaMM0oyQHDWX2wEfgpL2L0lYm-6yyW_OAhZ5jqPE7gXVI1TiF8o-fphdjuwR2JLZXhcVRLM0BbNLYLLmGjo--PWKqSR06iPn5GwDPvDyI8HXDXwVzo93vJcEw.eJ8-VDxkjdvzrES9ReOmFuj4j5di6HF2HTIwzSTGbhQ" xr:uid="{EDE7B70E-FEBC-406A-B39E-2AB503CA0144}"/>
+    <hyperlink ref="E63" r:id="rId42" xr:uid="{F4A25109-22B2-4774-8556-010A6432F45C}"/>
+    <hyperlink ref="E64" r:id="rId43" xr:uid="{56089546-10EB-4408-9A09-4DEBD7481848}"/>
+    <hyperlink ref="E19" r:id="rId44" xr:uid="{14589A0F-B504-4BE9-9AFE-5448BF150C87}"/>
+    <hyperlink ref="E40" r:id="rId45" xr:uid="{5723DA9D-D179-4AEB-AB95-294595786C74}"/>
+    <hyperlink ref="E41" r:id="rId46" xr:uid="{042DF449-509B-4AEA-9A35-77C1FB9C2735}"/>
+    <hyperlink ref="E44" r:id="rId47" xr:uid="{96328DC4-D284-4D83-BEF7-74DFDF600418}"/>
+    <hyperlink ref="E45" r:id="rId48" xr:uid="{DE36F8FF-4A6C-40BD-AAE6-2EED680C3898}"/>
+    <hyperlink ref="E46" r:id="rId49" xr:uid="{34A64F91-02F3-467E-BE15-CC86C3D830E3}"/>
+    <hyperlink ref="E47" r:id="rId50" xr:uid="{C7CFF23B-B4AD-4B40-AE34-2C736F0F2EEC}"/>
+    <hyperlink ref="E48" r:id="rId51" xr:uid="{D061E5B9-6B5D-4A8C-87DC-6AB1EFE918D9}"/>
+    <hyperlink ref="E49" r:id="rId52" xr:uid="{7E3C3772-744A-4671-863E-0AC0F3BC1DC4}"/>
+    <hyperlink ref="E50" r:id="rId53" xr:uid="{B7F14980-6546-4BA8-A7E9-12B0123B1973}"/>
+    <hyperlink ref="E65" r:id="rId54" xr:uid="{C03F301E-1DDE-43B9-96B0-8E626F826DD1}"/>
+    <hyperlink ref="E66" r:id="rId55" xr:uid="{C960EB57-8A4D-4F2C-B021-A2110DCDBFE6}"/>
+    <hyperlink ref="E67" r:id="rId56" xr:uid="{0F51C24B-5731-40DA-B3D9-7765B93C6025}"/>
+    <hyperlink ref="E68" r:id="rId57" xr:uid="{F267908B-A49A-4C91-A420-01096F7A73FB}"/>
+    <hyperlink ref="E69" r:id="rId58" xr:uid="{B16C09CA-B6D3-40FB-B5F6-0A74F113D147}"/>
+    <hyperlink ref="E70" r:id="rId59" xr:uid="{11FB9D27-1B25-4BD0-B30E-EA1605974124}"/>
+    <hyperlink ref="E71" r:id="rId60" xr:uid="{0D0EDC79-794C-4303-BD64-256E6390377A}"/>
+    <hyperlink ref="E72" r:id="rId61" xr:uid="{2CC32D6E-23AB-4957-BF43-727F4EEFCA7E}"/>
+    <hyperlink ref="E73" r:id="rId62" display="https://www.amazon.com/Miuzei-Waterproof-Compatible-Steering-Horn%EF%BC%88270%C2%B0%EF%BC%89/dp/B0C5LTKBD4?crid=2K8NLBN9K63XX&amp;dib=eyJ2IjoiMSJ9.n9l0Ww8Rh99Yx4hzyqJ9wSAyYPbGAZn5JMDhIOwhG3Uw9VdkAuhdsgHMtc7JHErXrmf3c268ZwFiHkeGe0ALflEUcg5wkIqvJz42MkQUS3bvyfMdTo_fCm8QV5itEJuxTHHOCoL7rykJ9owy7cODiUViszR0WHjpremcAmeUST13w_0mg2vkg4IgXuYQKZ7Ccs9oFabkHPIo3RM1o73uUMa3Behvkr31QSVdAIXbSvS7OLY_QLBOF2RP8fN9Xyg02z8P3gJxlLPofnqUuW03FaekBfju58afSh6dm8qpApI.WbTiyjsVeZwrAeYG6HzABV9sIZ-waYUxXiAkjk08HI8&amp;th=1" xr:uid="{1D0B1835-36B7-4E7A-848F-D949E2357CD4}"/>
+    <hyperlink ref="E74" r:id="rId63" display="https://www.amazon.com/Extension-Female-Connectors-Control-11-8In-15Pcs/dp/B0CG3CDQ94?crid=2081JSZ9MFZC1&amp;dib=eyJ2IjoiMSJ9.I7ZCJdlPJPsGhcKI302M1gm1hB9gbSQSY3NSu1xpA227bSCB24BUjDlVIGNF0ehsNOp8ZgfiAxO6nPkgPJidUHO6Fclu6tExIgcUKjUn2idqMO_uHKPGeZx9v9CaA0I2Juw_Fs4EiaU-4QZn82m0dlpbm3lBiUMpyrKhxjjBDDnv9wZVRSdjcYI37GiJM1Z8ESRUP8JmlbwT-exEMQZA0_nztRsRFG4qOIc5q5yEbHHTs0u8MraiDyI6jfmffO_vKCZB4cfFjDBUf9O3n2DpvBpkwN8pI-octMZbU1UVzT4.c_1Xt0QKON6To9mY2iIk-0Bfv5-USH13yYJAGg_KwBo" xr:uid="{3BA4891F-C4E0-4EBC-B725-FD3CC8460AC6}"/>
+    <hyperlink ref="E75" r:id="rId64" display="https://www.amazon.com/Splitter-Connector-Extension-Compatible-Airplanes/dp/B09VNQPP91?crid=3MAJU0RK53ZAK&amp;dib=eyJ2IjoiMSJ9.3gf6ef_DWLQUS_bMBdzBSTu4dobYQK0j9Fs4Xhy9Ud3t8GcEnYmE8bsj3X8Z8ztuwDi84HL1Owe9c_rKRE_Spg8NJxSfxbdVsp8QUMrwAsfNg_Ln4VQVY0Q0jP_r3rYiKjTouXB4jTmWD9bzZ4FsqbGN1H5RZUWxN05gVWIiDGqlFNU7xEPaMM0oyQHDWX2wEfgpL2L0lYm-6yyW_OAhZ5jqPE7gXVI1TiF8o-fphdjuwR2JLZXhcVRLM0BbNLYLLmGjo--PWKqSR06iPn5GwDPvDyI8HXDXwVzo93vJcEw.eJ8-VDxkjdvzrES9ReOmFuj4j5di6HF2HTIwzSTGbhQ" xr:uid="{EDE7B70E-FEBC-406A-B39E-2AB503CA0144}"/>
+    <hyperlink ref="E15" r:id="rId65" xr:uid="{BC43FF67-E3A1-4289-9B2D-4C958D0375AD}"/>
+    <hyperlink ref="E16" r:id="rId66" xr:uid="{3D8B6D06-0D56-43F7-8636-F78444433BE3}"/>
+    <hyperlink ref="E14" r:id="rId67" xr:uid="{383CF1DF-0BFE-4FE0-A3E2-C046A6F2B8F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId65"/>
+    <tablePart r:id="rId68"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4006,7 +4153,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:J15"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5258,7 +5405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9FF324-9493-4B86-8BE0-D1FA4EDEC6AF}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -5845,10 +5992,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F519261-6F0D-4794-9F6E-C24620020E68}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6405,42 +6552,117 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="C19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F19" s="2">
+        <v>34.86</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>34.86</v>
+      </c>
+      <c r="I19" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="A20" t="s">
+        <v>356</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C20" t="s">
+        <v>308</v>
+      </c>
+      <c r="D20" t="s">
+        <v>361</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="F20" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>358</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C21" t="s">
+        <v>308</v>
+      </c>
+      <c r="D21" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F21" s="2">
+        <v>38.72</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>38.72</v>
+      </c>
+      <c r="I21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="2">
-        <f>SUM(H2:H18)</f>
-        <v>223.16000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="F21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="2">
+        <f>SUM(H2:H21)</f>
+        <v>313.94000000000005</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F25" s="2"/>
-      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
@@ -6463,22 +6685,34 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="F31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B23:G23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -6506,7 +6740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A60099-C79D-465F-9791-AF166052DE65}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>